<commit_message>
neu file scan, pp
</commit_message>
<xml_diff>
--- a/DA2.3_DoanXuanThanh_517H0040_517H0093.xlsx
+++ b/DA2.3_DoanXuanThanh_517H0040_517H0093.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT Project\IT Project\IT-Project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFFB8F8-507A-4F8C-96BD-8B4AD1B99142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D566738-F61B-45B3-A6D7-5207395F59B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D4BD54A8-8A29-490D-AE46-455AD473DFA0}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>THÔNG TIN NHÓM SINH VIÊN</t>
   </si>
@@ -67,10 +67,6 @@
   </si>
   <si>
     <t>% hoàn thành</t>
-  </si>
-  <si>
-    <t>-
--….</t>
   </si>
   <si>
     <t>BÁO CÁO TIẾN ĐỘ GIỮA KỲ</t>
@@ -162,12 +158,102 @@
   <si>
     <t>Website quản lý tiến trình công việc cho các hoạt động của khoa CNTT</t>
   </si>
+  <si>
+    <t>Sửa lỗi và kiểm định ứng dụng</t>
+  </si>
+  <si>
+    <t>Kiểm định ứng dụng.
+Viết báo cáo, làm powerpoint thuyết trình</t>
+  </si>
+  <si>
+    <t>Khảo sát nhu cầu.
+Thiết kế, lên kế hoạch cho dự án.</t>
+  </si>
+  <si>
+    <t>Xây dựng khung dự án</t>
+  </si>
+  <si>
+    <t>Thiết kế ERD.
+Database
+Vẽ sơ lược UI hệ thông</t>
+  </si>
+  <si>
+    <t>Chọn công nghệ sử dụng.
+Và xây dựng cấu trúc tổng quát của dự án</t>
+  </si>
+  <si>
+    <t>Xây dựng model, database.
+Xây dựng API User.</t>
+  </si>
+  <si>
+    <t>Xây dựng model và database của User.
+CRUD của API User
+Xây dựng authenticate login api</t>
+  </si>
+  <si>
+    <t>Xây dựng model, database.
+Xây dựng API Event.</t>
+  </si>
+  <si>
+    <t>Xây dựng model và database của Events.
+CRUD của API Event.
+Các API tổng hợp dữ liệu của Events</t>
+  </si>
+  <si>
+    <t>Setup hệ thống gửi email.
+Xây dựng hệ thống gửi email thông báo tự đông</t>
+  </si>
+  <si>
+    <t>Setup hệ thống, thư viên gửi email.
+Xây dụng một job tự động gửi email thông báo cho người dùng về các sự kiên</t>
+  </si>
+  <si>
+    <t>Xây dựng trang "Login".
+Xây dựng phương thức đăng nhập bằng google account.
+Xây dựng trang "Dashboard".</t>
+  </si>
+  <si>
+    <t>Tiến hành dựng FE trang Login.
+Truyền dữ liệu từ google account tạo tài khoản mới, lưu vào hệ thống.
+Xây dụng và truyền dữ liệu tổng hợp sự kiện vào trang "Dashboard"</t>
+  </si>
+  <si>
+    <t>Xây dựng giao diện trang "Home".
+Xây dựng giao diện trang "Events"</t>
+  </si>
+  <si>
+    <t>Xây dựng giao diện trang "Home"
+2 tab Lịch và bảng trạng thái của hệ thống.
+Xây dựng giao diện trang "Events" và các phường thức thêm, xóa, sửa sự kiện.</t>
+  </si>
+  <si>
+    <t>Xây dựng trang "User".
+Xây dựng trang "Account".</t>
+  </si>
+  <si>
+    <t>Xây dựng giao diện trang "User".
+Xây dựng trang "Account".
+Và truyền dữ liệu các phương thức thêm, xóa, sửa, phân quyền người dùng trong hệ thống</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm mộ số phương thức lọc dữ liệu cho trang "Home", "User", "Event".
+Điều chỉnh giao diện Calendar.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thêm phương thức thêm học sinh đăng ký và học sinh tham gia bằng excel vào sự kiện.
+</t>
+  </si>
+  <si>
+    <t>Điều chỉnh UI, UX của hệ thống.
+Kiểm thử chức năng gửi email cho người dùng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +322,12 @@
       <family val="1"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -278,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,6 +405,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -327,9 +423,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -346,6 +444,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>243840</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>22861</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2827020</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F16FD538-8940-B49E-95A9-8C50513C7928}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7078980" y="17030701"/>
+          <a:ext cx="2583180" cy="1280159"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -650,25 +803,26 @@
   </sheetPr>
   <dimension ref="A1:Y1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="18.3984375" customWidth="1"/>
-    <col min="4" max="5" width="34.59765625" customWidth="1"/>
-    <col min="6" max="6" width="31.69921875" customWidth="1"/>
+    <col min="4" max="4" width="47" customWidth="1"/>
+    <col min="5" max="5" width="40.59765625" customWidth="1"/>
+    <col min="6" max="6" width="41.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="7" customFormat="1" ht="41.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>18</v>
+      <c r="A1" s="18" t="s">
+        <v>17</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -692,14 +846,14 @@
       <c r="Y1" s="6"/>
     </row>
     <row r="2" spans="1:25" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>20</v>
+      <c r="A2" s="19" t="s">
+        <v>19</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -749,11 +903,11 @@
     </row>
     <row r="4" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -782,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -809,12 +963,12 @@
     </row>
     <row r="6" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="19" t="s">
-        <v>26</v>
+      <c r="B6" s="21" t="s">
+        <v>25</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="20" t="s">
-        <v>22</v>
+      <c r="C6" s="21"/>
+      <c r="D6" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -841,12 +995,12 @@
     <row r="7" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -871,12 +1025,12 @@
     </row>
     <row r="8" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="19" t="s">
-        <v>25</v>
+      <c r="B8" s="21" t="s">
+        <v>24</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20" t="s">
-        <v>27</v>
+      <c r="C8" s="21"/>
+      <c r="D8" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -903,12 +1057,12 @@
     <row r="9" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -933,10 +1087,10 @@
     </row>
     <row r="10" spans="1:25" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -966,14 +1120,14 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1001,7 +1155,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1032,7 +1186,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1154,7 +1308,7 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="62.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>1</v>
       </c>
@@ -1165,13 +1319,13 @@
         <f>B17+6</f>
         <v>45263</v>
       </c>
-      <c r="D17" s="12" t="s">
-        <v>13</v>
+      <c r="D17" s="22" t="s">
+        <v>35</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>13</v>
+      <c r="E17" s="22" t="s">
+        <v>37</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="15">
         <v>1</v>
       </c>
       <c r="G17" s="2"/>
@@ -1194,7 +1348,7 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>2</v>
       </c>
@@ -1207,12 +1361,12 @@
         <v>45270</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>13</v>
+      <c r="E18" s="23" t="s">
+        <v>38</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="15">
         <v>1</v>
       </c>
       <c r="G18" s="2"/>
@@ -1235,7 +1389,7 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>3</v>
       </c>
@@ -1247,13 +1401,13 @@
         <f t="shared" si="0"/>
         <v>45277</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>13</v>
+      <c r="D19" s="22" t="s">
+        <v>39</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>13</v>
+      <c r="E19" s="22" t="s">
+        <v>40</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="15">
         <v>1</v>
       </c>
       <c r="G19" s="2"/>
@@ -1276,7 +1430,7 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="58.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>4</v>
       </c>
@@ -1288,13 +1442,13 @@
         <f t="shared" si="0"/>
         <v>45284</v>
       </c>
-      <c r="D20" s="12" t="s">
-        <v>13</v>
+      <c r="D20" s="22" t="s">
+        <v>41</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>13</v>
+      <c r="E20" s="22" t="s">
+        <v>42</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="15">
         <v>1</v>
       </c>
       <c r="G20" s="2"/>
@@ -1317,7 +1471,7 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>5</v>
       </c>
@@ -1329,13 +1483,13 @@
         <f t="shared" si="0"/>
         <v>45291</v>
       </c>
-      <c r="D21" s="12" t="s">
-        <v>13</v>
+      <c r="D21" s="22" t="s">
+        <v>43</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>13</v>
+      <c r="E21" s="22" t="s">
+        <v>44</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="15">
         <v>1</v>
       </c>
       <c r="G21" s="2"/>
@@ -1358,7 +1512,7 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="84" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>6</v>
       </c>
@@ -1370,13 +1524,13 @@
         <f t="shared" si="0"/>
         <v>45298</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>13</v>
+      <c r="D22" s="22" t="s">
+        <v>45</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>13</v>
+      <c r="E22" s="22" t="s">
+        <v>46</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="15">
         <v>1</v>
       </c>
       <c r="G22" s="2"/>
@@ -1399,7 +1553,7 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>7</v>
       </c>
@@ -1411,13 +1565,13 @@
         <f t="shared" si="0"/>
         <v>45305</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>13</v>
+      <c r="D23" s="22" t="s">
+        <v>47</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>13</v>
+      <c r="E23" s="22" t="s">
+        <v>48</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="15">
         <v>1</v>
       </c>
       <c r="G23" s="2"/>
@@ -1440,7 +1594,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="98.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>8</v>
       </c>
@@ -1452,13 +1606,13 @@
         <f t="shared" si="0"/>
         <v>45312</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>13</v>
+      <c r="D24" s="22" t="s">
+        <v>49</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>13</v>
+      <c r="E24" s="22" t="s">
+        <v>50</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="15">
         <v>1</v>
       </c>
       <c r="G24" s="2"/>
@@ -1481,7 +1635,7 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>9</v>
       </c>
@@ -1493,13 +1647,13 @@
         <f t="shared" si="0"/>
         <v>45319</v>
       </c>
-      <c r="D25" s="12" t="s">
-        <v>13</v>
+      <c r="D25" s="22" t="s">
+        <v>51</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>13</v>
+      <c r="E25" s="22" t="s">
+        <v>51</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="15">
         <v>1</v>
       </c>
       <c r="G25" s="2"/>
@@ -1534,11 +1688,11 @@
         <f t="shared" si="0"/>
         <v>45326</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>14</v>
+      <c r="D26" s="16" t="s">
+        <v>13</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1571,11 +1725,11 @@
         <f t="shared" si="0"/>
         <v>45333</v>
       </c>
-      <c r="D27" s="14" t="s">
-        <v>19</v>
+      <c r="D27" s="16" t="s">
+        <v>18</v>
       </c>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
@@ -1608,9 +1762,9 @@
         <f t="shared" si="0"/>
         <v>45340</v>
       </c>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
@@ -1631,7 +1785,7 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" ht="64.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>13</v>
       </c>
@@ -1643,13 +1797,13 @@
         <f t="shared" si="0"/>
         <v>45347</v>
       </c>
-      <c r="D29" s="12" t="s">
-        <v>13</v>
+      <c r="D29" s="22" t="s">
+        <v>52</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>13</v>
+      <c r="E29" s="22" t="s">
+        <v>52</v>
       </c>
-      <c r="F29" s="21">
+      <c r="F29" s="15">
         <v>1</v>
       </c>
       <c r="G29" s="2"/>
@@ -1672,7 +1826,7 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" ht="64.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>14</v>
       </c>
@@ -1684,13 +1838,13 @@
         <f t="shared" si="0"/>
         <v>45354</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>13</v>
+      <c r="D30" s="22" t="s">
+        <v>53</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>13</v>
+      <c r="E30" s="22" t="s">
+        <v>53</v>
       </c>
-      <c r="F30" s="21">
+      <c r="F30" s="15">
         <v>1</v>
       </c>
       <c r="G30" s="2"/>
@@ -1726,12 +1880,12 @@
         <v>45361</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="15">
         <v>1</v>
       </c>
       <c r="G31" s="2"/>
@@ -1754,7 +1908,7 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" ht="64.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>16</v>
       </c>
@@ -1766,13 +1920,13 @@
         <f t="shared" si="0"/>
         <v>45368</v>
       </c>
-      <c r="D32" s="12" t="s">
-        <v>13</v>
+      <c r="D32" s="22" t="s">
+        <v>34</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>13</v>
+      <c r="E32" s="22" t="s">
+        <v>34</v>
       </c>
-      <c r="F32" s="21">
+      <c r="F32" s="15">
         <v>1</v>
       </c>
       <c r="G32" s="2"/>
@@ -1807,11 +1961,11 @@
         <f t="shared" si="0"/>
         <v>45375</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>15</v>
+      <c r="D33" s="16" t="s">
+        <v>14</v>
       </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
@@ -1844,11 +1998,11 @@
         <f t="shared" si="0"/>
         <v>45382</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>16</v>
+      <c r="D34" s="16" t="s">
+        <v>15</v>
       </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
@@ -1897,12 +2051,12 @@
       <c r="Y35" s="2"/>
     </row>
     <row r="36" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="6"/>
       <c r="E36" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -28158,5 +28312,6 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.37" bottom="0.2" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="99" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>